<commit_message>
cl_base_new with new stopwords
Updated cl_base_new model with new stopwords and created new map
</commit_message>
<xml_diff>
--- a/classifier/topic-sdg_mapping.xlsx
+++ b/classifier/topic-sdg_mapping.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlafleur/Projects/SDGclassy/classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C4C0A2-2EF6-7B45-88B1-6FA5D3D522E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B483D0A9-8CF5-1D46-81E2-7C6F64DE6C83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="1240" windowWidth="27640" windowHeight="16540" xr2:uid="{C2E66343-9248-5B48-8AE3-7C7BC9517B48}"/>
+    <workbookView xWindow="1160" yWindow="1240" windowWidth="27640" windowHeight="16540" xr2:uid="{C2E66343-9248-5B48-8AE3-7C7BC9517B48}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -125,13 +125,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AAD20C-8106-C04B-8878-A00F42A6CDCF}">
-  <dimension ref="A3:K26"/>
+  <dimension ref="A3:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -468,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -493,8 +496,10 @@
       <c r="K4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -505,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -519,8 +524,9 @@
       <c r="K5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -531,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2">
         <v>2</v>
@@ -545,8 +551,9 @@
       <c r="K6">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -557,7 +564,7 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2">
         <v>3</v>
@@ -571,8 +578,9 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -597,8 +605,9 @@
       <c r="K8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -609,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2">
         <v>5</v>
@@ -623,8 +632,9 @@
       <c r="K9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -635,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2">
         <v>6</v>
@@ -649,8 +659,9 @@
       <c r="K10">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -661,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2">
         <v>7</v>
@@ -675,8 +686,9 @@
       <c r="K11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -687,7 +699,7 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2">
         <v>8</v>
@@ -701,8 +713,9 @@
       <c r="K12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -713,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G13" s="2">
         <v>9</v>
@@ -727,8 +740,9 @@
       <c r="K13">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -739,7 +753,7 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G14" s="2">
         <v>10</v>
@@ -753,8 +767,9 @@
       <c r="K14">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -765,7 +780,7 @@
         <v>11</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G15" s="2">
         <v>11</v>
@@ -779,8 +794,9 @@
       <c r="K15">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -791,7 +807,7 @@
         <v>12</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2">
         <v>12</v>
@@ -805,8 +821,9 @@
       <c r="K16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -817,7 +834,7 @@
         <v>13</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G17" s="2">
         <v>13</v>
@@ -831,8 +848,9 @@
       <c r="K17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -843,7 +861,7 @@
         <v>14</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G18" s="2">
         <v>14</v>
@@ -857,8 +875,9 @@
       <c r="K18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -869,7 +888,7 @@
         <v>15</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G19" s="2">
         <v>15</v>
@@ -883,8 +902,9 @@
       <c r="K19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -895,7 +915,7 @@
         <v>16</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G20" s="2">
         <v>16</v>
@@ -909,8 +929,9 @@
       <c r="K20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -921,7 +942,7 @@
         <v>17</v>
       </c>
       <c r="E21">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G21" s="2">
         <v>17</v>
@@ -935,8 +956,9 @@
       <c r="K21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -947,8 +969,8 @@
       <c r="D22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="3">
-        <v>12</v>
+      <c r="E22">
+        <v>8</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="5" t="s">
@@ -964,14 +986,15 @@
       <c r="K22" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -982,12 +1005,12 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>

</xml_diff>